<commit_message>
Added mapping for unmapped options
</commit_message>
<xml_diff>
--- a/scripts/old_data_migration_to_xml/FilesToRead/MappedExcel_PCMC/RA_Old_New_QuestionMapping_Parag.xlsx
+++ b/scripts/old_data_migration_to_xml/FilesToRead/MappedExcel_PCMC/RA_Old_New_QuestionMapping_Parag.xlsx
@@ -46,7 +46,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>available except pune city</t>
         </r>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3670" uniqueCount="1612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3671" uniqueCount="1612">
   <si>
     <t>begin_group</t>
   </si>
@@ -4889,17 +4889,17 @@
     <t>comments on gutters</t>
   </si>
   <si>
-    <t>1,2</t>
-  </si>
-  <si>
     <t>6,7</t>
+  </si>
+  <si>
+    <t>1,2,5,10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4910,7 +4910,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -4935,13 +4935,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <b/>
@@ -9461,8 +9454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M824"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E677" workbookViewId="0">
-      <selection activeCell="P517" sqref="P517"/>
+    <sheetView tabSelected="1" topLeftCell="A512" workbookViewId="0">
+      <selection activeCell="J524" sqref="J524"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16726,14 +16719,14 @@
         <v>407</v>
       </c>
       <c r="J517" s="14" t="s">
-        <v>1610</v>
+        <v>1611</v>
       </c>
       <c r="K517" s="27"/>
       <c r="L517" s="16">
         <v>256</v>
       </c>
       <c r="M517" s="14" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="518" spans="2:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -16874,8 +16867,8 @@
       <c r="I523" s="16">
         <v>407</v>
       </c>
-      <c r="J523" s="17">
-        <v>6</v>
+      <c r="J523" s="17" t="s">
+        <v>1610</v>
       </c>
       <c r="K523" s="27"/>
       <c r="L523" s="16">

</xml_diff>